<commit_message>
rebase pull commit 2?
</commit_message>
<xml_diff>
--- a/bdd/test.xlsx
+++ b/bdd/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>ID_sujeto</t>
   </si>
@@ -86,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -108,9 +108,6 @@
       <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
@@ -119,6 +116,7 @@
       <c r="B2" t="s" s="0">
         <v>6</v>
       </c>
+      <c r="D2" s="0"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
@@ -130,6 +128,7 @@
       <c r="C3" t="n" s="0">
         <v>0.0</v>
       </c>
+      <c r="D3" s="0"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
@@ -141,6 +140,7 @@
       <c r="C4" t="n" s="0">
         <v>1.0</v>
       </c>
+      <c r="D4" s="0"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
@@ -149,6 +149,7 @@
       <c r="B5" t="s" s="0">
         <v>6</v>
       </c>
+      <c r="D5" s="0"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
feat: servicio exportar excel completo y dicot. - Un poco de avances en criterios, todavía nada completamente funcional; falta lidiar con acciones específicas de las expresiones. - Limpiando el código de exportación un poco.
</commit_message>
<xml_diff>
--- a/bdd/test.xlsx
+++ b/bdd/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>ID_sujeto</t>
   </si>
@@ -86,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -108,9 +108,6 @@
       <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
@@ -119,6 +116,7 @@
       <c r="B2" t="s" s="0">
         <v>6</v>
       </c>
+      <c r="D2" s="0"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
@@ -130,6 +128,7 @@
       <c r="C3" t="n" s="0">
         <v>0.0</v>
       </c>
+      <c r="D3" s="0"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
@@ -141,6 +140,7 @@
       <c r="C4" t="n" s="0">
         <v>1.0</v>
       </c>
+      <c r="D4" s="0"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
@@ -149,6 +149,7 @@
       <c r="B5" t="s" s="0">
         <v>6</v>
       </c>
+      <c r="D5" s="0"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
feat: comentarios con leyendas en cada excel
</commit_message>
<xml_diff>
--- a/bdd/test.xlsx
+++ b/bdd/test.xlsx
@@ -11,8 +11,29 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+    <author>Leyenda</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="1">
+      <text>
+        <t>test 1</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="1">
+      <text>
+        <t>test 3</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>ID_sujeto</t>
   </si>
@@ -42,6 +63,12 @@
   </si>
   <si>
     <t>0004</t>
+  </si>
+  <si>
+    <t>0005</t>
+  </si>
+  <si>
+    <t>0006</t>
   </si>
 </sst>
 </file>
@@ -84,9 +111,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -151,7 +182,27 @@
       </c>
       <c r="D5" s="0"/>
     </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: comentarios con leyendas en cada excel v2 - se me olvidó los comentarios por criterio
</commit_message>
<xml_diff>
--- a/bdd/test.xlsx
+++ b/bdd/test.xlsx
@@ -21,6 +21,11 @@
     <comment ref="C1" authorId="1">
       <text>
         <t>test 1</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="1">
+      <text>
+        <t>test crit</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">

</xml_diff>

<commit_message>
feat: orden de columnas en excel por secciones - van ordenados de menor a mayor numero
</commit_message>
<xml_diff>
--- a/bdd/test.xlsx
+++ b/bdd/test.xlsx
@@ -20,15 +20,20 @@
   <commentList>
     <comment ref="C1" authorId="1">
       <text>
+        <t>testing secciones (seccion 0, debería ir primero)</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="1">
+      <text>
         <t>test 1</t>
       </text>
     </comment>
-    <comment ref="D1" authorId="1">
+    <comment ref="E1" authorId="1">
       <text>
         <t>test crit</t>
       </text>
     </comment>
-    <comment ref="E1" authorId="1">
+    <comment ref="F1" authorId="1">
       <text>
         <t>test 3</t>
       </text>
@@ -38,12 +43,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>ID_sujeto</t>
   </si>
   <si>
     <t>Tipo_sujeto</t>
+  </si>
+  <si>
+    <t>preg_secc0</t>
   </si>
   <si>
     <t>preg_test_1</t>
@@ -122,7 +130,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -144,66 +152,69 @@
       <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0"/>
+        <v>7</v>
+      </c>
+      <c r="E2" s="0"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n" s="0">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n" s="0">
         <v>0.0</v>
       </c>
-      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C4" t="n" s="0">
+        <v>7</v>
+      </c>
+      <c r="D4" t="n" s="0">
         <v>1.0</v>
       </c>
-      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0"/>
+        <v>7</v>
+      </c>
+      <c r="E5" s="0"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0"/>
+        <v>7</v>
+      </c>
+      <c r="E6" s="0"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D7" s="0"/>
+        <v>7</v>
+      </c>
+      <c r="E7" s="0"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
fix: criterios con datos de preguntas que no van al excel, ahora aparecen en la sección de la pregunta
</commit_message>
<xml_diff>
--- a/bdd/test.xlsx
+++ b/bdd/test.xlsx
@@ -35,6 +35,11 @@
     </comment>
     <comment ref="F1" authorId="1">
       <text>
+        <t>criterio con pregunta inexistente (en excel dicotomizado)</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="1">
+      <text>
         <t>test 3</t>
       </text>
     </comment>
@@ -43,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>ID_sujeto</t>
   </si>
@@ -58,6 +63,9 @@
   </si>
   <si>
     <t>nombre_stata_criterio1</t>
+  </si>
+  <si>
+    <t>crit_preg_inex</t>
   </si>
   <si>
     <t>pregunta_test_3</t>
@@ -130,7 +138,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -155,66 +163,75 @@
       <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
+      <c r="G1" t="s" s="0">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n" s="0">
         <v>1.0</v>
       </c>
       <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
feat: avance en calculo de criterios - por ahora debería calcularse todo criterio simple (val1 accion val2) si no se ocupa algo como la media o el promedio - no se si funciona el calculo de criterios con Y / O, no lo he testeado
</commit_message>
<xml_diff>
--- a/bdd/test.xlsx
+++ b/bdd/test.xlsx
@@ -25,20 +25,25 @@
     </comment>
     <comment ref="D1" authorId="1">
       <text>
+        <t>Criterio de preg_edad, donde es 1 si la respuesta es &lt;= 40</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="1">
+      <text>
         <t>test 1</t>
       </text>
     </comment>
-    <comment ref="E1" authorId="1">
+    <comment ref="F1" authorId="1">
       <text>
         <t>test crit</t>
       </text>
     </comment>
-    <comment ref="F1" authorId="1">
+    <comment ref="G1" authorId="1">
       <text>
         <t>criterio con pregunta inexistente (en excel dicotomizado)</t>
       </text>
     </comment>
-    <comment ref="G1" authorId="1">
+    <comment ref="H1" authorId="1">
       <text>
         <t>test 3</t>
       </text>
@@ -48,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>ID_sujeto</t>
   </si>
@@ -59,6 +64,9 @@
     <t>preg_secc0</t>
   </si>
   <si>
+    <t>crit_edad</t>
+  </si>
+  <si>
     <t>preg_test_1</t>
   </si>
   <si>
@@ -77,7 +85,13 @@
     <t>CO</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>0002</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>0003</t>
@@ -138,7 +152,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -166,72 +180,69 @@
       <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
+      <c r="H1" t="s" s="0">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
+        <v>9</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="D3" t="n" s="0">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E3" t="n">
         <v>0.0</v>
       </c>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="D4" t="n" s="0">
+        <v>9</v>
+      </c>
+      <c r="E4" t="n" s="0">
         <v>1.0</v>
       </c>
-      <c r="E4" s="0"/>
-      <c r="F4" s="0"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E5" s="0"/>
-      <c r="F5" s="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E6" s="0"/>
-      <c r="F6" s="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
feat: calculo de Promedio y media - calcula el promedio y la media de toda pregunta/dato numerico
</commit_message>
<xml_diff>
--- a/bdd/test.xlsx
+++ b/bdd/test.xlsx
@@ -30,20 +30,25 @@
     </comment>
     <comment ref="E1" authorId="1">
       <text>
+        <t>Criterio que es 1 si preg_edad es &gt; promedio (avg)</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="1">
+      <text>
         <t>test 1</t>
       </text>
     </comment>
-    <comment ref="F1" authorId="1">
+    <comment ref="G1" authorId="1">
       <text>
         <t>test crit</t>
       </text>
     </comment>
-    <comment ref="G1" authorId="1">
+    <comment ref="H1" authorId="1">
       <text>
         <t>criterio con pregunta inexistente (en excel dicotomizado)</t>
       </text>
     </comment>
-    <comment ref="H1" authorId="1">
+    <comment ref="I1" authorId="1">
       <text>
         <t>test 3</t>
       </text>
@@ -53,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>ID_sujeto</t>
   </si>
@@ -67,6 +72,9 @@
     <t>crit_edad</t>
   </si>
   <si>
+    <t>crit_edad_avg</t>
+  </si>
+  <si>
     <t>preg_test_1</t>
   </si>
   <si>
@@ -88,10 +96,10 @@
     <t>1</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>0002</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
   <si>
     <t>0003</t>
@@ -152,7 +160,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -183,65 +191,74 @@
       <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
+      <c r="I1" t="s" s="0">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E4" t="n" s="0">
+        <v>10</v>
+      </c>
+      <c r="F4" t="n" s="0">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: sumatoria de 0s y 1s en excel + algunos / eliminados para compatibilidad con docker
</commit_message>
<xml_diff>
--- a/bdd/test.xlsx
+++ b/bdd/test.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>ID_sujeto</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>0006</t>
+  </si>
+  <si>
+    <t>Cantidad de 0s =</t>
+  </si>
+  <si>
+    <t>Cantidad de 1s =</t>
   </si>
 </sst>
 </file>
@@ -160,7 +166,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -261,6 +267,58 @@
         <v>10</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C9" s="0">
+        <f>COUNTIF(C1:C7,1)</f>
+      </c>
+      <c r="D9" s="0">
+        <f>COUNTIF(D1:D7,1)</f>
+      </c>
+      <c r="E9" s="0">
+        <f>COUNTIF(E1:E7,1)</f>
+      </c>
+      <c r="F9" s="0">
+        <f>COUNTIF(F1:F7,1)</f>
+      </c>
+      <c r="G9" s="0">
+        <f>COUNTIF(G1:G7,1)</f>
+      </c>
+      <c r="H9" s="0">
+        <f>COUNTIF(H1:H7,1)</f>
+      </c>
+      <c r="I9" s="0">
+        <f>COUNTIF(I1:I7,1)</f>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C10" s="0">
+        <f>COUNTIF(C1:C7,0)</f>
+      </c>
+      <c r="D10" s="0">
+        <f>COUNTIF(D1:D7,0)</f>
+      </c>
+      <c r="E10" s="0">
+        <f>COUNTIF(E1:E7,0)</f>
+      </c>
+      <c r="F10" s="0">
+        <f>COUNTIF(F1:F7,0)</f>
+      </c>
+      <c r="G10" s="0">
+        <f>COUNTIF(G1:G7,0)</f>
+      </c>
+      <c r="H10" s="0">
+        <f>COUNTIF(H1:H7,0)</f>
+      </c>
+      <c r="I10" s="0">
+        <f>COUNTIF(I1:I7,0)</f>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
fix: resolución de errores con AND/OR, eliminar comentarios debug y preparación con getActivo()
</commit_message>
<xml_diff>
--- a/bdd/test.xlsx
+++ b/bdd/test.xlsx
@@ -35,20 +35,25 @@
     </comment>
     <comment ref="F1" authorId="1">
       <text>
+        <t>test criterio AND</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="1">
+      <text>
         <t>test 1</t>
       </text>
     </comment>
-    <comment ref="G1" authorId="1">
+    <comment ref="H1" authorId="1">
       <text>
         <t>test crit</t>
       </text>
     </comment>
-    <comment ref="H1" authorId="1">
+    <comment ref="I1" authorId="1">
       <text>
         <t>criterio con pregunta inexistente (en excel dicotomizado)</t>
       </text>
     </comment>
-    <comment ref="I1" authorId="1">
+    <comment ref="J1" authorId="1">
       <text>
         <t>test 3</t>
       </text>
@@ -58,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>ID_sujeto</t>
   </si>
@@ -73,6 +78,9 @@
   </si>
   <si>
     <t>crit_edad_avg</t>
+  </si>
+  <si>
+    <t>crit_and_test</t>
   </si>
   <si>
     <t>preg_test_1</t>
@@ -166,7 +174,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -200,76 +208,103 @@
       <c r="I1" t="s" s="0">
         <v>8</v>
       </c>
+      <c r="J1" t="s" s="0">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="n">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F4" t="n" s="0">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="0">
         <f>COUNTIF(C1:C7,1)</f>
@@ -292,10 +327,13 @@
       <c r="I9" s="0">
         <f>COUNTIF(I1:I7,1)</f>
       </c>
+      <c r="J9" s="0">
+        <f>COUNTIF(J1:J7,1)</f>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="0">
         <f>COUNTIF(C1:C7,0)</f>
@@ -317,6 +355,9 @@
       </c>
       <c r="I10" s="0">
         <f>COUNTIF(I1:I7,0)</f>
+      </c>
+      <c r="J10" s="0">
+        <f>COUNTIF(J1:J7,0)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>